<commit_message>
Continue working on what play types/codes indicate possession of ball
</commit_message>
<xml_diff>
--- a/Play_Poss_Indicators.xlsx
+++ b/Play_Poss_Indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="6720" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Who has ball" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="96">
   <si>
     <t>NA</t>
   </si>
@@ -282,6 +282,36 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Use Play Code, focus</t>
+  </si>
+  <si>
+    <t>Use type, focus</t>
+  </si>
+  <si>
+    <t>Use type, not focus</t>
+  </si>
+  <si>
+    <t>Next Play has ball</t>
+  </si>
+  <si>
+    <t>Prev Play has ball</t>
+  </si>
+  <si>
+    <t>prev_play</t>
+  </si>
+  <si>
+    <t>Play Code, prev play has ball</t>
+  </si>
+  <si>
+    <t>Play Code, next play has ball</t>
+  </si>
+  <si>
+    <t>Play Type, prev play has ball</t>
+  </si>
+  <si>
+    <t>Play Type, next play has ball</t>
   </si>
 </sst>
 </file>
@@ -366,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +426,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +729,7 @@
     <col min="5" max="6" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -711,6 +747,9 @@
       </c>
       <c r="F1" s="9" t="s">
         <v>80</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,6 +768,7 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -746,6 +786,9 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J3" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="L3" s="6" t="s">
         <v>79</v>
       </c>
@@ -770,6 +813,7 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J4" s="11"/>
       <c r="L4" s="7" t="s">
         <v>78</v>
       </c>
@@ -794,6 +838,7 @@
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J5" s="11"/>
       <c r="L5" s="7" t="s">
         <v>76</v>
       </c>
@@ -818,6 +863,7 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J6" s="11"/>
       <c r="L6" s="7" t="s">
         <v>75</v>
       </c>
@@ -842,6 +888,7 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J7" s="11"/>
       <c r="L7" s="7" t="s">
         <v>72</v>
       </c>
@@ -866,6 +913,7 @@
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J8" s="11"/>
       <c r="L8" s="7" t="s">
         <v>53</v>
       </c>
@@ -890,6 +938,7 @@
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J9" s="11"/>
       <c r="L9" s="7" t="s">
         <v>42</v>
       </c>
@@ -914,6 +963,7 @@
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J10" s="11"/>
       <c r="L10" s="7" t="s">
         <v>38</v>
       </c>
@@ -938,6 +988,7 @@
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J11" s="11"/>
       <c r="L11" s="7" t="s">
         <v>11</v>
       </c>
@@ -962,6 +1013,7 @@
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
@@ -979,6 +1031,9 @@
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J13" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="L13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1003,6 +1058,7 @@
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J14" s="11"/>
       <c r="L14" s="6" t="s">
         <v>62</v>
       </c>
@@ -1027,6 +1083,7 @@
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
@@ -1044,6 +1101,9 @@
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J16" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="L16" s="7" t="s">
         <v>69</v>
       </c>
@@ -1068,6 +1128,7 @@
       <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J17" s="11"/>
       <c r="L17" s="6" t="s">
         <v>68</v>
       </c>
@@ -1393,8 +1454,9 @@
       <c r="E32" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>47</v>
       </c>
@@ -1410,8 +1472,18 @@
       <c r="E33" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" ref="M33:M46" si="1">""""&amp;L33&amp;""""&amp;","</f>
+        <v>"jump_ball",</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>48</v>
       </c>
@@ -1427,8 +1499,15 @@
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="1"/>
+        <v>"period_start",</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>49</v>
       </c>
@@ -1444,8 +1523,9 @@
       <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>50</v>
       </c>
@@ -1461,8 +1541,18 @@
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="1"/>
+        <v>"period_end",</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>51</v>
       </c>
@@ -1478,8 +1568,9 @@
       <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>52</v>
       </c>
@@ -1495,8 +1586,18 @@
       <c r="E38" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>"AWAY_FROM_PLAY_FOUL",</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>54</v>
       </c>
@@ -1512,8 +1613,15 @@
       <c r="E39" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>"FLAGRANT_FOUL_TYPE_1",</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>55</v>
       </c>
@@ -1529,8 +1637,15 @@
       <c r="E40" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L40" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="1"/>
+        <v>"FOUL",</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>58</v>
       </c>
@@ -1546,8 +1661,15 @@
       <c r="E41" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="1"/>
+        <v>"LOOSE_BALL_FOUL",</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>59</v>
       </c>
@@ -1563,8 +1685,15 @@
       <c r="E42" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L42" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="1"/>
+        <v>"TECHNICAL_FOUL",</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>60</v>
       </c>
@@ -1580,8 +1709,15 @@
       <c r="E43" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="1"/>
+        <v>"DELAY_OF_GAME_VIOLATION",</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>61</v>
       </c>
@@ -1597,8 +1733,15 @@
       <c r="E44" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="1"/>
+        <v>"DOUBLE_LANE_VIOLATION",</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>62</v>
       </c>
@@ -1615,7 +1758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>63</v>
       </c>
@@ -1631,8 +1774,18 @@
       <c r="E46" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="1"/>
+        <v>"JUMP_BALL_VIOLATION",</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>64</v>
       </c>
@@ -1649,7 +1802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>65</v>
       </c>
@@ -1938,7 +2091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>22</v>
       </c>
@@ -1955,7 +2108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>23</v>
       </c>
@@ -1972,7 +2125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>16</v>
       </c>
@@ -1989,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>17</v>
       </c>
@@ -2006,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>20</v>
       </c>
@@ -2023,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>24</v>
       </c>
@@ -2040,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>25</v>
       </c>
@@ -2057,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>26</v>
       </c>
@@ -2074,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>27</v>
       </c>
@@ -2091,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>28</v>
       </c>
@@ -2108,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>82</v>
       </c>
@@ -2125,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>86</v>
       </c>
@@ -2142,7 +2295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>87</v>
       </c>
@@ -2159,133 +2312,160 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
+        <v>53</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="5">
+        <v>2005</v>
+      </c>
+      <c r="G78" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4">
+        <v>57</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="5">
+        <v>5009</v>
+      </c>
+      <c r="G79" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="4">
+        <v>85</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="5">
+        <v>169</v>
+      </c>
+      <c r="G80" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="4">
         <v>15</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D78" s="5">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="4">
-        <v>18</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D79" s="2">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="4">
-        <v>19</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D80" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="4">
-        <v>21</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C81" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D81" s="5">
+        <v>54</v>
+      </c>
+      <c r="G81" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="4">
+        <v>18</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="2">
+        <v>125</v>
+      </c>
+      <c r="G82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="4">
+        <v>19</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" s="5">
+        <v>1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="4">
+        <v>21</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="5">
+      <c r="D84" s="5">
         <v>2954</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4">
+      <c r="G84" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4">
         <v>29</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B85" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D82" s="5">
+      <c r="D85" s="5">
         <v>927</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="4">
-        <v>53</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83" s="8" t="s">
+      <c r="G85" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="4">
+        <v>56</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D83" s="5">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="4">
-        <v>88</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4">
-        <v>56</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D85" s="2">
+      <c r="D86" s="2">
         <v>5009</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="4">
-        <v>57</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D86" s="5">
-        <v>5009</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>83</v>
       </c>
@@ -2298,8 +2478,11 @@
       <c r="D87" s="5">
         <v>393</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>84</v>
       </c>
@@ -2312,23 +2495,26 @@
       <c r="D88" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
-        <v>85</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="5">
-        <v>169</v>
+        <v>88</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F89">
+  <sortState ref="A2:G89">
     <sortCondition ref="E2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete "Who has ball" possession calculations, clean up code.
</commit_message>
<xml_diff>
--- a/Play_Poss_Indicators.xlsx
+++ b/Play_Poss_Indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="8940" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Who has ball" sheetId="1" r:id="rId1"/>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38:M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1473,7 @@
         <v>9</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>40</v>
@@ -1542,7 +1542,7 @@
         <v>9</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L36" s="7" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Add possession summary block.
</commit_message>
<xml_diff>
--- a/Play_Poss_Indicators.xlsx
+++ b/Play_Poss_Indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Who has ball" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +346,15 @@
       <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +379,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -393,10 +405,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,8 +447,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -716,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38:M44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,6 +744,7 @@
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1034,7 +1052,7 @@
       <c r="J13" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M13" t="str">
@@ -1059,7 +1077,7 @@
         <v>9</v>
       </c>
       <c r="J14" s="11"/>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="13" t="s">
         <v>62</v>
       </c>
       <c r="M14" t="str">
@@ -1084,6 +1102,13 @@
         <v>9</v>
       </c>
       <c r="J15" s="11"/>
+      <c r="L15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="str">
+        <f>""""&amp;L15&amp;""""&amp;","</f>
+        <v>"SHOOTING_FOUL",</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
@@ -1101,16 +1126,6 @@
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="0"/>
-        <v>"CLEAR_PATH_FOUL",</v>
-      </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
@@ -1128,13 +1143,15 @@
       <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="L17" s="6" t="s">
-        <v>68</v>
+      <c r="J17" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
-        <v>"DEF_3_SEC_TECH_FOUL",</v>
+        <v>"CLEAR_PATH_FOUL",</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1153,12 +1170,12 @@
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>65</v>
+      <c r="L18" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
-        <v>"INBOUND_FOUL",</v>
+        <v>"DEF_3_SEC_TECH_FOUL",</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1177,12 +1194,12 @@
       <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>61</v>
+      <c r="L19" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
-        <v>"PERSONAL_BLOCK_FOUL",</v>
+        <v>"INBOUND_FOUL",</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1201,12 +1218,12 @@
       <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>60</v>
+      <c r="L20" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
-        <v>"PERSONAL_FOUL",</v>
+        <v>"PERSONAL_BLOCK_FOUL",</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1225,12 +1242,12 @@
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="7" t="s">
-        <v>59</v>
+      <c r="L21" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
-        <v>"PERSONAL_TAKE_FOUL",</v>
+        <v>"PERSONAL_FOUL",</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,12 +1266,12 @@
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="6" t="s">
-        <v>58</v>
+      <c r="L22" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
-        <v>"SHOOTING_BLOCK_FOUL",</v>
+        <v>"PERSONAL_TAKE_FOUL",</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1273,12 +1290,12 @@
       <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>57</v>
+      <c r="L23" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
-        <v>"SHOOTING_FOUL",</v>
+        <v>"SHOOTING_BLOCK_FOUL",</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1297,7 +1314,7 @@
       <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="13" t="s">
         <v>8</v>
       </c>
       <c r="M24" t="str">
@@ -1321,7 +1338,7 @@
       <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="13" t="s">
         <v>4</v>
       </c>
       <c r="M25" t="str">
@@ -1345,7 +1362,7 @@
       <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="13" t="s">
         <v>2</v>
       </c>
       <c r="M26" t="str">

</xml_diff>